<commit_message>
update text cleaning strings
</commit_message>
<xml_diff>
--- a/methods_dictionary.xlsx
+++ b/methods_dictionary.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/whitenm_qut_edu_au/Documents/Git projects/stats_section/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{187F6103-615A-47C5-BA3D-1C61B4FE5D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{187F6103-615A-47C5-BA3D-1C61B4FE5D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55DCC982-A84A-473A-B5A3-F2C354DDCFBC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6941413E-72A1-4783-89A4-EE179FBDE9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="stats_terms" sheetId="1" r:id="rId1"/>
-    <sheet name="uk_spelling" sheetId="3" r:id="rId2"/>
+    <sheet name="other" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -501,9 +501,6 @@
     <t xml:space="preserve">burn in </t>
   </si>
   <si>
-    <t>burn-in-</t>
-  </si>
-  <si>
     <t>metropolis hastings</t>
   </si>
   <si>
@@ -636,9 +633,6 @@
     <t>regression</t>
   </si>
   <si>
-    <t>kmean</t>
-  </si>
-  <si>
     <t>fisher</t>
   </si>
   <si>
@@ -931,6 +925,12 @@
   </si>
   <si>
     <t>two-sided</t>
+  </si>
+  <si>
+    <t>burn-in</t>
+  </si>
+  <si>
+    <t>k-mean</t>
   </si>
 </sst>
 </file>
@@ -1296,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85770F85-B2D3-4508-9B12-71AB5E6420BB}">
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,18 +1315,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1339,42 +1339,42 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1435,34 +1435,34 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B20" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1478,7 +1478,7 @@
         <v>154</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>155</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1515,58 +1515,58 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B31" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B33" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1579,10 +1579,10 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B35" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1598,7 +1598,7 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1611,18 +1611,18 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1638,7 +1638,7 @@
         <v>127</v>
       </c>
       <c r="B42" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1659,18 +1659,18 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B45" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B46" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1691,18 +1691,18 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B49" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B50" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1715,42 +1715,42 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B52" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B53" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B55" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B56" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1758,23 +1758,23 @@
         <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B58" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B59" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1835,10 +1835,10 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B67" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1851,10 +1851,10 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B69" t="s">
-        <v>200</v>
+        <v>298</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1867,34 +1867,34 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B71" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B72" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1966,31 +1966,31 @@
         <v>51</v>
       </c>
       <c r="B83" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B84" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B85" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1998,7 +1998,7 @@
         <v>44</v>
       </c>
       <c r="B87" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2006,7 +2006,7 @@
         <v>45</v>
       </c>
       <c r="B88" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>45</v>
       </c>
       <c r="B89" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2022,7 +2022,7 @@
         <v>48</v>
       </c>
       <c r="B90" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2030,23 +2030,23 @@
         <v>49</v>
       </c>
       <c r="B91" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2054,15 +2054,15 @@
         <v>50</v>
       </c>
       <c r="B94" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B95" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2094,15 +2094,15 @@
         <v>52</v>
       </c>
       <c r="B99" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B100" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2150,7 +2150,7 @@
         <v>54</v>
       </c>
       <c r="B106" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2182,7 +2182,7 @@
         <v>56</v>
       </c>
       <c r="B110" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2203,18 +2203,18 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B113" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2235,34 +2235,34 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B117" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B118" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B119" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B120" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2275,10 +2275,10 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B122" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2307,18 +2307,18 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B126" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B127" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2326,15 +2326,15 @@
         <v>53</v>
       </c>
       <c r="B128" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B129" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2395,18 +2395,18 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B137" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B138" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2475,7 +2475,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,138 +2494,138 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B12" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B15" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B16" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B17" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B18" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>